<commit_message>
will calculate granulation / oscillation / activity noise floor
</commit_message>
<xml_diff>
--- a/results/GAIA__TESS_candidate__matches__unique_stars.xlsx
+++ b/results/GAIA__TESS_candidate__matches__unique_stars.xlsx
@@ -2173,7 +2173,7 @@
         </is>
       </c>
       <c r="AC15" t="n">
-        <v>21.38573457164645</v>
+        <v>21.38573457164644</v>
       </c>
       <c r="AD15" t="inlineStr">
         <is>
@@ -2728,7 +2728,7 @@
         </is>
       </c>
       <c r="AC20" t="n">
-        <v>23.73536925404753</v>
+        <v>23.73536925404754</v>
       </c>
       <c r="AD20" t="inlineStr">
         <is>
@@ -3371,7 +3371,7 @@
         </is>
       </c>
       <c r="AC26" t="n">
-        <v>36.96574143989465</v>
+        <v>36.96574143989464</v>
       </c>
       <c r="AD26" t="inlineStr">
         <is>
@@ -4116,7 +4116,7 @@
         </is>
       </c>
       <c r="AC33" t="n">
-        <v>31.58870948768593</v>
+        <v>31.58870948768594</v>
       </c>
       <c r="AD33" t="inlineStr">
         <is>
@@ -4225,7 +4225,7 @@
         </is>
       </c>
       <c r="AC34" t="n">
-        <v>38.943923431253</v>
+        <v>38.94392343125299</v>
       </c>
       <c r="AD34" t="inlineStr">
         <is>
@@ -4871,7 +4871,7 @@
         </is>
       </c>
       <c r="AC40" t="n">
-        <v>46.06148963783664</v>
+        <v>46.06148963783663</v>
       </c>
       <c r="AD40" t="inlineStr">
         <is>
@@ -4980,7 +4980,7 @@
         </is>
       </c>
       <c r="AC41" t="n">
-        <v>39.09037625797879</v>
+        <v>39.0903762579788</v>
       </c>
       <c r="AD41" t="inlineStr">
         <is>
@@ -5517,7 +5517,7 @@
         </is>
       </c>
       <c r="AC46" t="n">
-        <v>45.59948147549512</v>
+        <v>45.5994814754951</v>
       </c>
       <c r="AD46" t="inlineStr">
         <is>
@@ -5626,7 +5626,7 @@
         </is>
       </c>
       <c r="AC47" t="n">
-        <v>47.77434230850001</v>
+        <v>47.7743423085</v>
       </c>
       <c r="AD47" t="inlineStr">
         <is>
@@ -5828,7 +5828,7 @@
         </is>
       </c>
       <c r="AC49" t="n">
-        <v>49.36973911725026</v>
+        <v>49.36973911725025</v>
       </c>
       <c r="AD49" t="inlineStr">
         <is>
@@ -5932,7 +5932,7 @@
         </is>
       </c>
       <c r="AC50" t="n">
-        <v>44.85630836711914</v>
+        <v>44.85630836711915</v>
       </c>
       <c r="AD50" t="inlineStr">
         <is>
@@ -6754,7 +6754,7 @@
         </is>
       </c>
       <c r="AC58" t="n">
-        <v>40.09106465613873</v>
+        <v>40.09106465613874</v>
       </c>
       <c r="AD58" t="inlineStr">
         <is>
@@ -6847,7 +6847,7 @@
         </is>
       </c>
       <c r="AC59" t="n">
-        <v>41.80344952411276</v>
+        <v>41.80344952411277</v>
       </c>
       <c r="AD59" t="inlineStr">
         <is>
@@ -7254,7 +7254,7 @@
         </is>
       </c>
       <c r="AC63" t="n">
-        <v>42.42813356345498</v>
+        <v>42.42813356345499</v>
       </c>
       <c r="AD63" t="inlineStr">
         <is>
@@ -7539,7 +7539,7 @@
         </is>
       </c>
       <c r="AC66" t="n">
-        <v>43.07406530599914</v>
+        <v>43.07406530599913</v>
       </c>
       <c r="AD66" t="inlineStr">
         <is>
@@ -7648,7 +7648,7 @@
         </is>
       </c>
       <c r="AC67" t="n">
-        <v>31.70399233689045</v>
+        <v>31.70399233689044</v>
       </c>
       <c r="AD67" t="inlineStr">
         <is>
@@ -7757,7 +7757,7 @@
         </is>
       </c>
       <c r="AC68" t="n">
-        <v>45.18455781418142</v>
+        <v>45.18455781418143</v>
       </c>
       <c r="AD68" t="inlineStr">
         <is>
@@ -7866,7 +7866,7 @@
         </is>
       </c>
       <c r="AC69" t="n">
-        <v>33.92840645115611</v>
+        <v>33.92840645115612</v>
       </c>
       <c r="AD69" t="inlineStr">
         <is>

</xml_diff>